<commit_message>
Refactor the code #1 - Final
</commit_message>
<xml_diff>
--- a/Resources/testdata.xlsx
+++ b/Resources/testdata.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\way2automation\PycharmProjects\RobotFrameworkProject\Resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\samfi\PycharmProjects\Robot_Framework\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D979463-698C-483E-AB3C-0D2AF4FC1FBC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C4741F1-3A13-42AA-A099-E1297005A8F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{7618D423-091D-4ED8-98E2-F0664639E4A7}"/>
+    <workbookView xWindow="-100" yWindow="-100" windowWidth="21467" windowHeight="11443" xr2:uid="{7618D423-091D-4ED8-98E2-F0664639E4A7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -438,16 +438,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C35C65C6-3C0B-49B8-8C59-D409E32DC40B}">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.09765625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -455,7 +455,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -463,7 +463,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -471,7 +471,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -479,7 +479,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -496,13 +496,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50E20EF2-669F-4E14-81C9-6C149F07571B}">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>14</v>
       </c>
@@ -513,7 +513,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -524,7 +524,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -535,7 +535,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>6</v>
       </c>

</xml_diff>

<commit_message>
Adding the Data Driven Test
</commit_message>
<xml_diff>
--- a/Resources/testdata.xlsx
+++ b/Resources/testdata.xlsx
@@ -1,40 +1,32 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\samfi\PycharmProjects\Robot_Framework\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C4741F1-3A13-42AA-A099-E1297005A8F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5622D41E-882F-494F-8EB9-511A0261A305}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-100" yWindow="-100" windowWidth="21467" windowHeight="11443" xr2:uid="{7618D423-091D-4ED8-98E2-F0664639E4A7}"/>
+    <workbookView xWindow="-100" yWindow="-100" windowWidth="21467" windowHeight="11443" activeTab="1" xr2:uid="{7618D423-091D-4ED8-98E2-F0664639E4A7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="FindNewCarTest" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="23">
   <si>
     <t>${month}</t>
   </si>
@@ -54,37 +46,55 @@
     <t>December</t>
   </si>
   <si>
+    <t>toyota</t>
+  </si>
+  <si>
+    <t>kia</t>
+  </si>
+  <si>
+    <t>bmw</t>
+  </si>
+  <si>
+    <t>Kia Cars</t>
+  </si>
+  <si>
+    <t>BMW Cars</t>
+  </si>
+  <si>
+    <t>Toyota Cars</t>
+  </si>
+  <si>
+    <t>${browser}</t>
+  </si>
+  <si>
+    <t>${brandname}</t>
+  </si>
+  <si>
+    <t>${carheading}</t>
+  </si>
+  <si>
+    <t>tata</t>
+  </si>
+  <si>
+    <t>Tata Cars</t>
+  </si>
+  <si>
+    <t>firefox</t>
+  </si>
+  <si>
     <t>chrome</t>
   </si>
   <si>
-    <t>firefox</t>
-  </si>
-  <si>
-    <t>toyota</t>
-  </si>
-  <si>
-    <t>kia</t>
-  </si>
-  <si>
-    <t>bmw</t>
-  </si>
-  <si>
-    <t>Kia Cars</t>
-  </si>
-  <si>
-    <t>BMW Cars</t>
-  </si>
-  <si>
-    <t>Toyota Cars</t>
-  </si>
-  <si>
-    <t>${browser}</t>
-  </si>
-  <si>
-    <t>${brandname}</t>
-  </si>
-  <si>
-    <t>${carheading}</t>
+    <t>maruti</t>
+  </si>
+  <si>
+    <t>Maruti Cars</t>
+  </si>
+  <si>
+    <t>honda</t>
+  </si>
+  <si>
+    <t>Honda Cars</t>
   </si>
 </sst>
 </file>
@@ -438,7 +448,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C35C65C6-3C0B-49B8-8C59-D409E32DC40B}">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
@@ -494,56 +504,89 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50E20EF2-669F-4E14-81C9-6C149F07571B}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" t="s">
         <v>14</v>
-      </c>
-      <c r="B1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C1" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" t="s">
         <v>6</v>
       </c>
-      <c r="B2" t="s">
-        <v>8</v>
-      </c>
       <c r="C2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" t="s">
         <v>7</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>9</v>
-      </c>
-      <c r="C3" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" t="s">
         <v>10</v>
       </c>
-      <c r="C4" t="s">
-        <v>12</v>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>